<commit_message>
feat: Updated logic when uploading cases to perfomer queue and some fixes for stability
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Rakel Meddelanden och Bilagor Performer Dispatcher</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1654,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1840,8 +1843,8 @@
       <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="b">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>38</v>

</xml_diff>